<commit_message>
edit for multi-prize lottery system.
</commit_message>
<xml_diff>
--- a/CubicDraw/WorkBooks/NameList.xlsx
+++ b/CubicDraw/WorkBooks/NameList.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C64BE8EB-7506-4E4F-B5F2-B3EA241D05CF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE7FECEA-0560-4DDA-A7E3-55A887603022}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1128" yWindow="-108" windowWidth="22020" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,43 +20,319 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>老大</t>
-  </si>
-  <si>
-    <t>张三</t>
-  </si>
-  <si>
-    <t>李四</t>
-  </si>
-  <si>
-    <t>王五</t>
-  </si>
-  <si>
-    <t>肥宅</t>
-  </si>
-  <si>
-    <t>老赵</t>
-  </si>
-  <si>
-    <t>老李</t>
-  </si>
-  <si>
-    <t>意大利炮</t>
-  </si>
-  <si>
-    <t>秀芹</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="99">
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>69</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>73</t>
+  </si>
+  <si>
+    <t>74</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>76</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>78</t>
+  </si>
+  <si>
+    <t>79</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>81</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>83</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>85</t>
+  </si>
+  <si>
+    <t>86</t>
+  </si>
+  <si>
+    <t>87</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>89</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>91</t>
+  </si>
+  <si>
+    <t>92</t>
+  </si>
+  <si>
+    <t>93</t>
+  </si>
+  <si>
+    <t>94</t>
+  </si>
+  <si>
+    <t>95</t>
+  </si>
+  <si>
+    <t>96</t>
+  </si>
+  <si>
+    <t>97</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>99</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -365,15 +641,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" style="1" customWidth="1"/>
     <col min="2" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
@@ -422,7 +698,458 @@
         <v>8</v>
       </c>
     </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A92" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A94" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A95" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A96" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A97" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A98" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A99" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
ambient and attenuation changed, with logo3 modified.
</commit_message>
<xml_diff>
--- a/CubicDraw/WorkBooks/NameList.xlsx
+++ b/CubicDraw/WorkBooks/NameList.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE7FECEA-0560-4DDA-A7E3-55A887603022}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA5D244-579A-4C14-A7E0-7A071D49C5F7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1128" yWindow="-108" windowWidth="22020" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,303 +20,456 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="99">
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>39</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>41</t>
-  </si>
-  <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>43</t>
-  </si>
-  <si>
-    <t>44</t>
-  </si>
-  <si>
-    <t>45</t>
-  </si>
-  <si>
-    <t>46</t>
-  </si>
-  <si>
-    <t>47</t>
-  </si>
-  <si>
-    <t>48</t>
-  </si>
-  <si>
-    <t>49</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>51</t>
-  </si>
-  <si>
-    <t>52</t>
-  </si>
-  <si>
-    <t>53</t>
-  </si>
-  <si>
-    <t>54</t>
-  </si>
-  <si>
-    <t>55</t>
-  </si>
-  <si>
-    <t>56</t>
-  </si>
-  <si>
-    <t>57</t>
-  </si>
-  <si>
-    <t>58</t>
-  </si>
-  <si>
-    <t>59</t>
-  </si>
-  <si>
-    <t>60</t>
-  </si>
-  <si>
-    <t>61</t>
-  </si>
-  <si>
-    <t>62</t>
-  </si>
-  <si>
-    <t>63</t>
-  </si>
-  <si>
-    <t>64</t>
-  </si>
-  <si>
-    <t>65</t>
-  </si>
-  <si>
-    <t>66</t>
-  </si>
-  <si>
-    <t>67</t>
-  </si>
-  <si>
-    <t>68</t>
-  </si>
-  <si>
-    <t>69</t>
-  </si>
-  <si>
-    <t>70</t>
-  </si>
-  <si>
-    <t>71</t>
-  </si>
-  <si>
-    <t>72</t>
-  </si>
-  <si>
-    <t>73</t>
-  </si>
-  <si>
-    <t>74</t>
-  </si>
-  <si>
-    <t>75</t>
-  </si>
-  <si>
-    <t>76</t>
-  </si>
-  <si>
-    <t>77</t>
-  </si>
-  <si>
-    <t>78</t>
-  </si>
-  <si>
-    <t>79</t>
-  </si>
-  <si>
-    <t>80</t>
-  </si>
-  <si>
-    <t>81</t>
-  </si>
-  <si>
-    <t>82</t>
-  </si>
-  <si>
-    <t>83</t>
-  </si>
-  <si>
-    <t>84</t>
-  </si>
-  <si>
-    <t>85</t>
-  </si>
-  <si>
-    <t>86</t>
-  </si>
-  <si>
-    <t>87</t>
-  </si>
-  <si>
-    <t>88</t>
-  </si>
-  <si>
-    <t>89</t>
-  </si>
-  <si>
-    <t>90</t>
-  </si>
-  <si>
-    <t>91</t>
-  </si>
-  <si>
-    <t>92</t>
-  </si>
-  <si>
-    <t>93</t>
-  </si>
-  <si>
-    <t>94</t>
-  </si>
-  <si>
-    <t>95</t>
-  </si>
-  <si>
-    <t>96</t>
-  </si>
-  <si>
-    <t>97</t>
-  </si>
-  <si>
-    <t>98</t>
-  </si>
-  <si>
-    <t>99</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="150">
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>002</t>
+  </si>
+  <si>
+    <t>003</t>
+  </si>
+  <si>
+    <t>004</t>
+  </si>
+  <si>
+    <t>005</t>
+  </si>
+  <si>
+    <t>006</t>
+  </si>
+  <si>
+    <t>007</t>
+  </si>
+  <si>
+    <t>008</t>
+  </si>
+  <si>
+    <t>009</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>011</t>
+  </si>
+  <si>
+    <t>012</t>
+  </si>
+  <si>
+    <t>013</t>
+  </si>
+  <si>
+    <t>014</t>
+  </si>
+  <si>
+    <t>015</t>
+  </si>
+  <si>
+    <t>016</t>
+  </si>
+  <si>
+    <t>017</t>
+  </si>
+  <si>
+    <t>018</t>
+  </si>
+  <si>
+    <t>019</t>
+  </si>
+  <si>
+    <t>020</t>
+  </si>
+  <si>
+    <t>021</t>
+  </si>
+  <si>
+    <t>022</t>
+  </si>
+  <si>
+    <t>023</t>
+  </si>
+  <si>
+    <t>024</t>
+  </si>
+  <si>
+    <t>025</t>
+  </si>
+  <si>
+    <t>026</t>
+  </si>
+  <si>
+    <t>027</t>
+  </si>
+  <si>
+    <t>028</t>
+  </si>
+  <si>
+    <t>029</t>
+  </si>
+  <si>
+    <t>030</t>
+  </si>
+  <si>
+    <t>031</t>
+  </si>
+  <si>
+    <t>032</t>
+  </si>
+  <si>
+    <t>033</t>
+  </si>
+  <si>
+    <t>034</t>
+  </si>
+  <si>
+    <t>035</t>
+  </si>
+  <si>
+    <t>036</t>
+  </si>
+  <si>
+    <t>037</t>
+  </si>
+  <si>
+    <t>038</t>
+  </si>
+  <si>
+    <t>039</t>
+  </si>
+  <si>
+    <t>040</t>
+  </si>
+  <si>
+    <t>041</t>
+  </si>
+  <si>
+    <t>042</t>
+  </si>
+  <si>
+    <t>043</t>
+  </si>
+  <si>
+    <t>044</t>
+  </si>
+  <si>
+    <t>045</t>
+  </si>
+  <si>
+    <t>046</t>
+  </si>
+  <si>
+    <t>047</t>
+  </si>
+  <si>
+    <t>048</t>
+  </si>
+  <si>
+    <t>049</t>
+  </si>
+  <si>
+    <t>050</t>
+  </si>
+  <si>
+    <t>051</t>
+  </si>
+  <si>
+    <t>052</t>
+  </si>
+  <si>
+    <t>053</t>
+  </si>
+  <si>
+    <t>054</t>
+  </si>
+  <si>
+    <t>055</t>
+  </si>
+  <si>
+    <t>056</t>
+  </si>
+  <si>
+    <t>057</t>
+  </si>
+  <si>
+    <t>058</t>
+  </si>
+  <si>
+    <t>059</t>
+  </si>
+  <si>
+    <t>060</t>
+  </si>
+  <si>
+    <t>061</t>
+  </si>
+  <si>
+    <t>062</t>
+  </si>
+  <si>
+    <t>063</t>
+  </si>
+  <si>
+    <t>064</t>
+  </si>
+  <si>
+    <t>065</t>
+  </si>
+  <si>
+    <t>066</t>
+  </si>
+  <si>
+    <t>067</t>
+  </si>
+  <si>
+    <t>068</t>
+  </si>
+  <si>
+    <t>069</t>
+  </si>
+  <si>
+    <t>070</t>
+  </si>
+  <si>
+    <t>071</t>
+  </si>
+  <si>
+    <t>072</t>
+  </si>
+  <si>
+    <t>073</t>
+  </si>
+  <si>
+    <t>074</t>
+  </si>
+  <si>
+    <t>075</t>
+  </si>
+  <si>
+    <t>076</t>
+  </si>
+  <si>
+    <t>077</t>
+  </si>
+  <si>
+    <t>078</t>
+  </si>
+  <si>
+    <t>079</t>
+  </si>
+  <si>
+    <t>080</t>
+  </si>
+  <si>
+    <t>081</t>
+  </si>
+  <si>
+    <t>082</t>
+  </si>
+  <si>
+    <t>083</t>
+  </si>
+  <si>
+    <t>084</t>
+  </si>
+  <si>
+    <t>085</t>
+  </si>
+  <si>
+    <t>086</t>
+  </si>
+  <si>
+    <t>087</t>
+  </si>
+  <si>
+    <t>088</t>
+  </si>
+  <si>
+    <t>089</t>
+  </si>
+  <si>
+    <t>090</t>
+  </si>
+  <si>
+    <t>091</t>
+  </si>
+  <si>
+    <t>092</t>
+  </si>
+  <si>
+    <t>093</t>
+  </si>
+  <si>
+    <t>094</t>
+  </si>
+  <si>
+    <t>095</t>
+  </si>
+  <si>
+    <t>096</t>
+  </si>
+  <si>
+    <t>097</t>
+  </si>
+  <si>
+    <t>098</t>
+  </si>
+  <si>
+    <t>099</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>102</t>
+  </si>
+  <si>
+    <t>103</t>
+  </si>
+  <si>
+    <t>104</t>
+  </si>
+  <si>
+    <t>105</t>
+  </si>
+  <si>
+    <t>106</t>
+  </si>
+  <si>
+    <t>107</t>
+  </si>
+  <si>
+    <t>108</t>
+  </si>
+  <si>
+    <t>109</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>112</t>
+  </si>
+  <si>
+    <t>113</t>
+  </si>
+  <si>
+    <t>114</t>
+  </si>
+  <si>
+    <t>115</t>
+  </si>
+  <si>
+    <t>116</t>
+  </si>
+  <si>
+    <t>117</t>
+  </si>
+  <si>
+    <t>118</t>
+  </si>
+  <si>
+    <t>119</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>121</t>
+  </si>
+  <si>
+    <t>122</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>124</t>
+  </si>
+  <si>
+    <t>125</t>
+  </si>
+  <si>
+    <t>126</t>
+  </si>
+  <si>
+    <t>127</t>
+  </si>
+  <si>
+    <t>128</t>
+  </si>
+  <si>
+    <t>129</t>
+  </si>
+  <si>
+    <t>130</t>
+  </si>
+  <si>
+    <t>131</t>
+  </si>
+  <si>
+    <t>132</t>
+  </si>
+  <si>
+    <t>133</t>
+  </si>
+  <si>
+    <t>134</t>
+  </si>
+  <si>
+    <t>135</t>
+  </si>
+  <si>
+    <t>136</t>
+  </si>
+  <si>
+    <t>137</t>
+  </si>
+  <si>
+    <t>138</t>
+  </si>
+  <si>
+    <t>139</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>141</t>
+  </si>
+  <si>
+    <t>142</t>
+  </si>
+  <si>
+    <t>143</t>
+  </si>
+  <si>
+    <t>144</t>
+  </si>
+  <si>
+    <t>145</t>
+  </si>
+  <si>
+    <t>146</t>
+  </si>
+  <si>
+    <t>147</t>
+  </si>
+  <si>
+    <t>148</t>
+  </si>
+  <si>
+    <t>149</t>
+  </si>
+  <si>
+    <t>150</t>
   </si>
 </sst>
 </file>
@@ -641,15 +794,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A99"/>
+  <dimension ref="A1:A150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="D96" sqref="D96"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" style="1" customWidth="1"/>
     <col min="2" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
@@ -1148,6 +1301,261 @@
         <v>98</v>
       </c>
     </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A100" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A101" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A102" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A103" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A104" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A105" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A106" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A107" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A108" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A109" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A110" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A111" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A112" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A113" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A114" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A115" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A116" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A117" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A118" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A119" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A120" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A121" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A122" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A123" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A124" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A125" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A126" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A127" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A128" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A129" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A130" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A131" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A132" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A133" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A134" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A135" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A136" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A137" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A138" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A139" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A140" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A141" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A142" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A143" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A144" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A145" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A146" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A147" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A148" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A149" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A150" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>